<commit_message>
editing tables and ms
</commit_message>
<xml_diff>
--- a/ms/nature communications ms/Supplementary/Supplementary_model tables_S1-S8.xlsx
+++ b/ms/nature communications ms/Supplementary/Supplementary_model tables_S1-S8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/nature communications ms/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_diff_meta/ms/nature communications ms/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C161144D-F827-594C-B837-54222A06A2C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF626EE-F44B-CF41-9BC8-B1B77C8025FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="460" windowWidth="36020" windowHeight="19760" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="529">
   <si>
     <t>Birds</t>
   </si>
@@ -455,9 +455,6 @@
     <t>-0.56, 0.69</t>
   </si>
   <si>
-    <t>-0.70, 0.74</t>
-  </si>
-  <si>
     <t>-1.10, 1.31</t>
   </si>
   <si>
@@ -527,36 +524,6 @@
     <t>-3.18, 2.92</t>
   </si>
   <si>
-    <t>-0.38, 0.32</t>
-  </si>
-  <si>
-    <t>0.07, 1.04</t>
-  </si>
-  <si>
-    <t>0.00, 0.69</t>
-  </si>
-  <si>
-    <t>-0.31, 0.58</t>
-  </si>
-  <si>
-    <t>-0.40, 0.87</t>
-  </si>
-  <si>
-    <t>-1.86, 0.62</t>
-  </si>
-  <si>
-    <t>-1.67, 1.77</t>
-  </si>
-  <si>
-    <t>-0.06, 2.30</t>
-  </si>
-  <si>
-    <t>-0.52, 3.41</t>
-  </si>
-  <si>
-    <t>-5.57, 5.08</t>
-  </si>
-  <si>
     <t>-0.61, 0.50</t>
   </si>
   <si>
@@ -626,33 +593,6 @@
     <t>-2.24, 2.64</t>
   </si>
   <si>
-    <t>p=0.45</t>
-  </si>
-  <si>
-    <t>-0.18, 0.08</t>
-  </si>
-  <si>
-    <t>-0.12, 0.11</t>
-  </si>
-  <si>
-    <t>-0.18, 0.58</t>
-  </si>
-  <si>
-    <t>-0.47, 0.64</t>
-  </si>
-  <si>
-    <t>-0.14, 1.56</t>
-  </si>
-  <si>
-    <t>-0.66, 0.68</t>
-  </si>
-  <si>
-    <t>-1.61, 0.88</t>
-  </si>
-  <si>
-    <t>-4.08, 2.93</t>
-  </si>
-  <si>
     <t>-0.39, 0.90</t>
   </si>
   <si>
@@ -743,57 +683,6 @@
     <t>-2.32, 2.71</t>
   </si>
   <si>
-    <t>-2.16, 2.10</t>
-  </si>
-  <si>
-    <t>-1.60, 2.71</t>
-  </si>
-  <si>
-    <t>-1.78, 2.47</t>
-  </si>
-  <si>
-    <t>-2.01, 2.28</t>
-  </si>
-  <si>
-    <t>-1.96, 2.43</t>
-  </si>
-  <si>
-    <t>-2.66, 2.76</t>
-  </si>
-  <si>
-    <t>-1.29, 3.52</t>
-  </si>
-  <si>
-    <t>-1.43, 4.32</t>
-  </si>
-  <si>
-    <t>-5.97, 4.32</t>
-  </si>
-  <si>
-    <t>-0.76, 0.66</t>
-  </si>
-  <si>
-    <t>-0.72, 0.70</t>
-  </si>
-  <si>
-    <t>-0.70, 0.75</t>
-  </si>
-  <si>
-    <t>-0.60, 0.99</t>
-  </si>
-  <si>
-    <t>-0.39, 1.81</t>
-  </si>
-  <si>
-    <t>-0.95, 0.98</t>
-  </si>
-  <si>
-    <t>-1.79, 1.06</t>
-  </si>
-  <si>
-    <t>-4.15, 3.00</t>
-  </si>
-  <si>
     <t>-1.24, 1.53</t>
   </si>
   <si>
@@ -1599,6 +1488,138 @@
   </si>
   <si>
     <t>Supplementary Tables for Harrison et al. 2020 - Part A, S1-S8</t>
+  </si>
+  <si>
+    <t>p=0.62</t>
+  </si>
+  <si>
+    <t>-0.19, 0.13</t>
+  </si>
+  <si>
+    <t>-0.16, 0.11</t>
+  </si>
+  <si>
+    <t>-0.27, 0.35</t>
+  </si>
+  <si>
+    <t>-0.14, 0.70</t>
+  </si>
+  <si>
+    <t>-0.44, 0.79</t>
+  </si>
+  <si>
+    <t>-0.60, 1.94</t>
+  </si>
+  <si>
+    <t>-0.82, 0.67</t>
+  </si>
+  <si>
+    <t>-2.06, 1.38</t>
+  </si>
+  <si>
+    <t>-0.25, 0.57</t>
+  </si>
+  <si>
+    <t>-0.50, 1.55</t>
+  </si>
+  <si>
+    <t>-0.10, 0.72</t>
+  </si>
+  <si>
+    <t>-0.85, 0.55</t>
+  </si>
+  <si>
+    <t>-0.56, 1.01</t>
+  </si>
+  <si>
+    <t>-2.25, 0.51</t>
+  </si>
+  <si>
+    <t>-2.82, 5.44</t>
+  </si>
+  <si>
+    <t>-0.31, 2.41</t>
+  </si>
+  <si>
+    <t>-2.74, 3.16</t>
+  </si>
+  <si>
+    <t>-2.14, 2.46</t>
+  </si>
+  <si>
+    <t>-1.96, 3.01</t>
+  </si>
+  <si>
+    <t>-1.99, 2.61</t>
+  </si>
+  <si>
+    <t>-2.52, 2.22</t>
+  </si>
+  <si>
+    <t>-2.17, 2.62</t>
+  </si>
+  <si>
+    <t>-3.40, 6.02</t>
+  </si>
+  <si>
+    <t>-1.59, 3.69</t>
+  </si>
+  <si>
+    <t>-3.51, 3.93</t>
+  </si>
+  <si>
+    <t>-0.80, 0.75</t>
+  </si>
+  <si>
+    <t>-0.80, 0.85</t>
+  </si>
+  <si>
+    <t>-0.79, 0.74</t>
+  </si>
+  <si>
+    <t>-0.78, 0.86</t>
+  </si>
+  <si>
+    <t>-0.58, 1.15</t>
+  </si>
+  <si>
+    <t>-0.81, 2.15</t>
+  </si>
+  <si>
+    <t>-1.14, 0.99</t>
+  </si>
+  <si>
+    <t>-2.22, 1.54</t>
+  </si>
+  <si>
+    <t>-0.25, 0.17</t>
+  </si>
+  <si>
+    <t>-0.53, 1.07</t>
+  </si>
+  <si>
+    <t>p=0.50</t>
+  </si>
+  <si>
+    <t>p=0.41</t>
+  </si>
+  <si>
+    <t>-0.42, 1.04</t>
+  </si>
+  <si>
+    <t>-2.26, 0.93</t>
+  </si>
+  <si>
+    <t>p=0.95</t>
+  </si>
+  <si>
+    <t>-0.47, 0.51</t>
+  </si>
+  <si>
+    <t>-0.03, 0.38</t>
+  </si>
+  <si>
+    <t>-0.54, 1.10</t>
   </si>
 </sst>
 </file>
@@ -2088,119 +2109,119 @@
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>521</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>480</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>482</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>481</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>483</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>326</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>301</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>304</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>325</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2212,7 +2233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAF7C5E-35C2-0343-8AC1-0E9A3B22FC74}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -2227,23 +2248,23 @@
   <sheetData>
     <row r="1" spans="1:34" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -2502,7 +2523,7 @@
         <v>0.73</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>470</v>
+        <v>433</v>
       </c>
       <c r="F10">
         <v>50</v>
@@ -2538,7 +2559,7 @@
         <v>0.7</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>472</v>
+        <v>435</v>
       </c>
       <c r="T10">
         <v>37</v>
@@ -2556,7 +2577,7 @@
         <v>0.23</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>476</v>
+        <v>439</v>
       </c>
       <c r="AA10">
         <v>61</v>
@@ -2769,7 +2790,7 @@
         <v>0.24</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="AC13" t="s">
         <v>16</v>
@@ -2789,7 +2810,7 @@
         <v>0.93</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>471</v>
+        <v>434</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
@@ -2886,7 +2907,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>19</v>
@@ -2903,7 +2924,7 @@
         <v>22</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="M16" s="9" t="s">
         <v>19</v>
@@ -2920,7 +2941,7 @@
         <v>22</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="T16" s="9" t="s">
         <v>19</v>
@@ -2937,7 +2958,7 @@
         <v>22</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AA16" s="9" t="s">
         <v>19</v>
@@ -2954,7 +2975,7 @@
         <v>22</v>
       </c>
       <c r="AG16" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AH16" s="9" t="s">
         <v>19</v>
@@ -2966,13 +2987,13 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>332</v>
+        <v>295</v>
       </c>
       <c r="D17" s="3">
         <v>-1.17</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>327</v>
+        <v>290</v>
       </c>
       <c r="F17" s="3">
         <v>0.24</v>
@@ -3004,13 +3025,13 @@
         <v>0.3</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>447</v>
+        <v>410</v>
       </c>
       <c r="R17" s="3">
         <v>1.82</v>
       </c>
       <c r="S17" s="33" t="s">
-        <v>478</v>
+        <v>441</v>
       </c>
       <c r="T17" s="3">
         <v>7.0000000000000007E-2</v>
@@ -3303,7 +3324,7 @@
         <v>0.2</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>473</v>
+        <v>436</v>
       </c>
       <c r="T22">
         <v>37</v>
@@ -3321,7 +3342,7 @@
         <v>0.17</v>
       </c>
       <c r="Z22" t="s">
-        <v>477</v>
+        <v>440</v>
       </c>
       <c r="AA22">
         <v>61</v>
@@ -3359,7 +3380,7 @@
         <v>0.44</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="F23">
         <v>106</v>
@@ -3531,7 +3552,7 @@
         <v>0.02</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
       <c r="V25" s="5" t="s">
         <v>16</v>
@@ -3540,7 +3561,7 @@
         <v>0.43</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>336</v>
+        <v>299</v>
       </c>
       <c r="AC25" s="5" t="s">
         <v>16</v>
@@ -3560,7 +3581,7 @@
         <v>0.94</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="H26" t="s">
         <v>17</v>
@@ -3578,7 +3599,7 @@
         <v>0.76</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>475</v>
+        <v>438</v>
       </c>
       <c r="V26" t="s">
         <v>17</v>
@@ -3587,7 +3608,7 @@
         <v>0.6</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="AC26" t="s">
         <v>17</v>
@@ -3657,7 +3678,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>19</v>
@@ -3674,7 +3695,7 @@
         <v>22</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>19</v>
@@ -3691,7 +3712,7 @@
         <v>22</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="T28" s="9" t="s">
         <v>19</v>
@@ -3708,7 +3729,7 @@
         <v>22</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AA28" s="9" t="s">
         <v>19</v>
@@ -3725,7 +3746,7 @@
         <v>22</v>
       </c>
       <c r="AG28" s="8" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AH28" s="9" t="s">
         <v>19</v>
@@ -3737,13 +3758,13 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="D29" s="3">
         <v>-0.56000000000000005</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>328</v>
+        <v>291</v>
       </c>
       <c r="F29" s="3">
         <v>0.57999999999999996</v>
@@ -3775,13 +3796,13 @@
         <v>0</v>
       </c>
       <c r="Q29" s="33" t="s">
-        <v>469</v>
+        <v>432</v>
       </c>
       <c r="R29" s="3">
         <v>-0.04</v>
       </c>
       <c r="S29" s="33" t="s">
-        <v>479</v>
+        <v>442</v>
       </c>
       <c r="T29" s="3">
         <v>0.97</v>
@@ -3794,7 +3815,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="X29" s="33" t="s">
-        <v>334</v>
+        <v>297</v>
       </c>
       <c r="Y29" s="3">
         <v>0.51</v>
@@ -4022,7 +4043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF86D62B-22BF-1846-B677-968C777627E8}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="N2" workbookViewId="0">
       <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
@@ -4037,23 +4058,23 @@
   <sheetData>
     <row r="1" spans="1:45" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>313</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:45" s="11" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4185,7 +4206,7 @@
         <v>3.76</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -4628,7 +4649,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>22</v>
@@ -4653,7 +4674,7 @@
         <v>33</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>22</v>
@@ -4678,7 +4699,7 @@
         <v>33</v>
       </c>
       <c r="V15" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="W15" s="8" t="s">
         <v>22</v>
@@ -4703,7 +4724,7 @@
         <v>33</v>
       </c>
       <c r="AE15" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AF15" s="8" t="s">
         <v>22</v>
@@ -4728,7 +4749,7 @@
         <v>33</v>
       </c>
       <c r="AN15" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AO15" s="8" t="s">
         <v>22</v>
@@ -4754,10 +4775,10 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="E16">
         <v>-0.93</v>
@@ -4808,10 +4829,10 @@
         <v>0.33</v>
       </c>
       <c r="U16" s="23" t="s">
-        <v>448</v>
+        <v>411</v>
       </c>
       <c r="V16" s="23" t="s">
-        <v>462</v>
+        <v>425</v>
       </c>
       <c r="W16">
         <v>1.77</v>
@@ -4838,7 +4859,7 @@
         <v>106</v>
       </c>
       <c r="AE16" s="23" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="AF16">
         <v>-0.84</v>
@@ -4865,7 +4886,7 @@
         <v>45</v>
       </c>
       <c r="AN16" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AO16">
         <v>-0.23</v>
@@ -4891,10 +4912,10 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>341</v>
+        <v>304</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="E17">
         <v>-0.97</v>
@@ -4945,10 +4966,10 @@
         <v>0.35</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>449</v>
+        <v>412</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>463</v>
+        <v>426</v>
       </c>
       <c r="W17" s="5">
         <v>0.97</v>
@@ -4975,7 +4996,7 @@
         <v>107</v>
       </c>
       <c r="AE17" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AF17" s="5">
         <v>0.55000000000000004</v>
@@ -5002,7 +5023,7 @@
         <v>110</v>
       </c>
       <c r="AN17" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AO17">
         <v>-0.52</v>
@@ -5028,10 +5049,10 @@
         <v>-0.19</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>342</v>
+        <v>305</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>368</v>
+        <v>331</v>
       </c>
       <c r="E18">
         <v>-1.5</v>
@@ -5082,10 +5103,10 @@
         <v>0.31</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>450</v>
+        <v>413</v>
       </c>
       <c r="V18" s="36" t="s">
-        <v>464</v>
+        <v>427</v>
       </c>
       <c r="W18" s="5">
         <v>1.7</v>
@@ -5112,7 +5133,7 @@
         <v>108</v>
       </c>
       <c r="AE18" s="36" t="s">
-        <v>364</v>
+        <v>327</v>
       </c>
       <c r="AF18" s="5">
         <v>0.85</v>
@@ -5139,7 +5160,7 @@
         <v>111</v>
       </c>
       <c r="AN18" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AO18">
         <v>1.1100000000000001</v>
@@ -5165,10 +5186,10 @@
         <v>0.09</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>343</v>
+        <v>306</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>369</v>
+        <v>332</v>
       </c>
       <c r="E19">
         <v>0.66</v>
@@ -5219,10 +5240,10 @@
         <v>0</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>451</v>
+        <v>414</v>
       </c>
       <c r="V19" s="35" t="s">
-        <v>465</v>
+        <v>428</v>
       </c>
       <c r="W19">
         <v>0.02</v>
@@ -5246,10 +5267,10 @@
         <v>0.05</v>
       </c>
       <c r="AD19" s="24" t="s">
-        <v>344</v>
+        <v>307</v>
       </c>
       <c r="AE19" s="36" t="s">
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="AF19" s="5">
         <v>0.26</v>
@@ -5276,7 +5297,7 @@
         <v>112</v>
       </c>
       <c r="AN19" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AO19" s="4">
         <v>2.44</v>
@@ -5356,10 +5377,10 @@
         <v>0.39</v>
       </c>
       <c r="U20" s="27" t="s">
-        <v>452</v>
+        <v>415</v>
       </c>
       <c r="V20" s="27" t="s">
-        <v>466</v>
+        <v>429</v>
       </c>
       <c r="W20" s="16">
         <v>1</v>
@@ -5386,7 +5407,7 @@
         <v>109</v>
       </c>
       <c r="AE20" s="25" t="s">
-        <v>366</v>
+        <v>329</v>
       </c>
       <c r="AF20" s="15">
         <v>0.46</v>
@@ -5413,7 +5434,7 @@
         <v>113</v>
       </c>
       <c r="AN20" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AO20" s="16">
         <v>-0.18</v>
@@ -5503,7 +5524,7 @@
         <v>1.17</v>
       </c>
       <c r="C23" t="s">
-        <v>345</v>
+        <v>308</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
@@ -5527,7 +5548,7 @@
         <v>1.03</v>
       </c>
       <c r="U23" s="5" t="s">
-        <v>467</v>
+        <v>430</v>
       </c>
       <c r="V23" s="5" t="s">
         <v>39</v>
@@ -5539,7 +5560,7 @@
         <v>0.26</v>
       </c>
       <c r="AD23" t="s">
-        <v>349</v>
+        <v>312</v>
       </c>
       <c r="AE23" t="s">
         <v>39</v>
@@ -5944,7 +5965,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>22</v>
@@ -5968,7 +5989,7 @@
         <v>33</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="N30" s="17" t="s">
         <v>22</v>
@@ -5992,7 +6013,7 @@
         <v>33</v>
       </c>
       <c r="V30" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="W30" s="17" t="s">
         <v>22</v>
@@ -6016,7 +6037,7 @@
         <v>33</v>
       </c>
       <c r="AE30" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AF30" s="17" t="s">
         <v>22</v>
@@ -6040,7 +6061,7 @@
         <v>33</v>
       </c>
       <c r="AN30" s="9" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="AO30" s="17" t="s">
         <v>22</v>
@@ -6069,7 +6090,7 @@
         <v>121</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="E31" s="7">
         <v>0.36</v>
@@ -6120,10 +6141,10 @@
         <v>-0.06</v>
       </c>
       <c r="U31" s="31" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
       <c r="V31" s="23" t="s">
-        <v>457</v>
+        <v>420</v>
       </c>
       <c r="W31" s="21">
         <v>-0.83</v>
@@ -6147,10 +6168,10 @@
         <v>0.1</v>
       </c>
       <c r="AD31" s="28" t="s">
-        <v>350</v>
+        <v>313</v>
       </c>
       <c r="AE31" s="28" t="s">
-        <v>354</v>
+        <v>317</v>
       </c>
       <c r="AF31" s="7">
         <v>0.67</v>
@@ -6177,7 +6198,7 @@
         <v>124</v>
       </c>
       <c r="AN31" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AO31" s="7">
         <v>-0.53</v>
@@ -6203,10 +6224,10 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>359</v>
+        <v>322</v>
       </c>
       <c r="E32" s="18">
         <v>-0.41</v>
@@ -6257,10 +6278,10 @@
         <v>0.17</v>
       </c>
       <c r="U32" s="32" t="s">
-        <v>454</v>
+        <v>417</v>
       </c>
       <c r="V32" s="23" t="s">
-        <v>458</v>
+        <v>421</v>
       </c>
       <c r="W32" s="18">
         <v>1.22</v>
@@ -6287,7 +6308,7 @@
         <v>120</v>
       </c>
       <c r="AE32" s="32" t="s">
-        <v>354</v>
+        <v>317</v>
       </c>
       <c r="AF32" s="18">
         <v>0.69</v>
@@ -6314,7 +6335,7 @@
         <v>125</v>
       </c>
       <c r="AN32" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AO32" s="22">
         <v>1.73</v>
@@ -6340,10 +6361,10 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>346</v>
+        <v>309</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="E33" s="18">
         <v>-0.04</v>
@@ -6394,10 +6415,10 @@
         <v>-0.04</v>
       </c>
       <c r="U33" s="32" t="s">
-        <v>468</v>
+        <v>431</v>
       </c>
       <c r="V33" s="35" t="s">
-        <v>459</v>
+        <v>422</v>
       </c>
       <c r="W33" s="18">
         <v>-0.61</v>
@@ -6421,10 +6442,10 @@
         <v>0.06</v>
       </c>
       <c r="AD33" s="32" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
       <c r="AE33" s="35" t="s">
-        <v>355</v>
+        <v>318</v>
       </c>
       <c r="AF33" s="18">
         <v>0.43</v>
@@ -6451,7 +6472,7 @@
         <v>126</v>
       </c>
       <c r="AN33" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AO33" s="18">
         <v>0.83</v>
@@ -6477,10 +6498,10 @@
         <v>-0.25</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>347</v>
+        <v>310</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="E34" s="22">
         <v>-1.92</v>
@@ -6531,10 +6552,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U34" s="32" t="s">
-        <v>455</v>
+        <v>418</v>
       </c>
       <c r="V34" s="35" t="s">
-        <v>460</v>
+        <v>423</v>
       </c>
       <c r="W34" s="18">
         <v>0.73</v>
@@ -6558,10 +6579,10 @@
         <v>0.04</v>
       </c>
       <c r="AD34" s="32" t="s">
-        <v>352</v>
+        <v>315</v>
       </c>
       <c r="AE34" s="35" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="AF34" s="18">
         <v>0.28000000000000003</v>
@@ -6588,7 +6609,7 @@
         <v>127</v>
       </c>
       <c r="AN34" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AO34" s="18">
         <v>-0.84</v>
@@ -6614,10 +6635,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>348</v>
+        <v>311</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>362</v>
+        <v>325</v>
       </c>
       <c r="E35" s="16">
         <v>0.53</v>
@@ -6668,10 +6689,10 @@
         <v>0.27</v>
       </c>
       <c r="U35" s="27" t="s">
-        <v>456</v>
+        <v>419</v>
       </c>
       <c r="V35" s="27" t="s">
-        <v>461</v>
+        <v>424</v>
       </c>
       <c r="W35" s="16">
         <v>1.29</v>
@@ -6695,10 +6716,10 @@
         <v>0.06</v>
       </c>
       <c r="AD35" s="27" t="s">
-        <v>353</v>
+        <v>316</v>
       </c>
       <c r="AE35" s="27" t="s">
-        <v>357</v>
+        <v>320</v>
       </c>
       <c r="AF35" s="16">
         <v>0.39</v>
@@ -6725,7 +6746,7 @@
         <v>128</v>
       </c>
       <c r="AN35" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AO35" s="16">
         <v>-0.38</v>
@@ -6753,7 +6774,7 @@
   <dimension ref="A1:AW97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="X11" sqref="X11:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6773,13 +6794,13 @@
   <sheetData>
     <row r="1" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>312</v>
+        <v>275</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>307</v>
+        <v>270</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="43"/>
@@ -6832,7 +6853,7 @@
     </row>
     <row r="3" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>271</v>
       </c>
       <c r="B3"/>
       <c r="K3" s="19"/>
@@ -6842,7 +6863,7 @@
     </row>
     <row r="4" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>306</v>
+        <v>269</v>
       </c>
       <c r="B4"/>
       <c r="K4" s="22"/>
@@ -6951,7 +6972,7 @@
         <v>23</v>
       </c>
       <c r="V7" s="5">
-        <v>2801.44</v>
+        <v>2608.44</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>7</v>
@@ -6972,7 +6993,7 @@
         <v>136.65</v>
       </c>
       <c r="AQ7" s="5" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:49" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -6983,7 +7004,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>105</v>
@@ -6995,22 +7016,22 @@
         <v>1</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="U8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="V8" s="4">
-        <v>2.13</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>68</v>
+      <c r="V8" s="5">
+        <v>1.23</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="AE8" s="4" t="s">
         <v>36</v>
@@ -7208,13 +7229,13 @@
         <v>12</v>
       </c>
       <c r="V11" s="5">
-        <v>0.89</v>
+        <v>1.02</v>
       </c>
       <c r="W11" s="5">
-        <v>0.94</v>
+        <v>1.01</v>
       </c>
       <c r="X11" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AE11" s="5" t="s">
         <v>12</v>
@@ -7273,10 +7294,10 @@
         <v>0</v>
       </c>
       <c r="W12" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="X12" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AE12" s="5" t="s">
         <v>50</v>
@@ -7332,13 +7353,13 @@
         <v>15</v>
       </c>
       <c r="V13" s="5">
-        <v>0.26</v>
+        <v>0.3</v>
       </c>
       <c r="W13" s="5">
-        <v>0.51</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X13" s="5">
-        <v>481</v>
+        <v>420</v>
       </c>
       <c r="AE13" s="5" t="s">
         <v>15</v>
@@ -7565,13 +7586,13 @@
         <v>-0.16</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D16" s="5">
         <v>-1.02</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F16" s="5">
         <v>0.31</v>
@@ -7592,13 +7613,13 @@
         <v>-0.11</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N16" s="5">
         <v>-0.39</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="P16" s="5">
         <v>0.7</v>
@@ -7616,28 +7637,28 @@
         <v>27</v>
       </c>
       <c r="V16" s="5">
-        <v>-0.03</v>
+        <v>0.16</v>
       </c>
       <c r="W16" s="24" t="s">
-        <v>164</v>
+        <v>494</v>
       </c>
       <c r="X16" s="5">
-        <v>-0.18</v>
+        <v>0.76</v>
       </c>
       <c r="Y16" s="24" t="s">
-        <v>236</v>
+        <v>503</v>
       </c>
       <c r="Z16" s="5">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="AA16" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AB16" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC16" s="5">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="AE16" s="5" t="s">
         <v>27</v>
@@ -7646,13 +7667,13 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AG16" s="24" t="s">
-        <v>378</v>
+        <v>341</v>
       </c>
       <c r="AH16" s="5">
         <v>0.47</v>
       </c>
       <c r="AI16" s="24" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="AJ16" s="5">
         <v>0.64</v>
@@ -7673,13 +7694,13 @@
         <v>0</v>
       </c>
       <c r="AQ16" s="24" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="AR16" s="5">
         <v>0</v>
       </c>
       <c r="AS16" s="24" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="AT16" s="5">
         <v>1</v>
@@ -7702,13 +7723,13 @@
         <v>-0.15</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>370</v>
+        <v>333</v>
       </c>
       <c r="D17" s="5">
         <v>-0.96</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>402</v>
+        <v>365</v>
       </c>
       <c r="F17" s="5">
         <v>0.34</v>
@@ -7729,13 +7750,13 @@
         <v>-0.06</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N17" s="5">
         <v>-0.24</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="P17" s="5">
         <v>0.81</v>
@@ -7749,32 +7770,32 @@
       <c r="S17" s="5">
         <v>93</v>
       </c>
-      <c r="U17" s="4" t="s">
+      <c r="U17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="V17" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="W17" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="X17" s="4">
-        <v>2.23</v>
-      </c>
-      <c r="Y17" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z17" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="AA17" s="4">
-        <v>9</v>
-      </c>
-      <c r="AB17" s="4">
-        <v>9</v>
-      </c>
-      <c r="AC17" s="4">
-        <v>44</v>
+      <c r="V17" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="W17" s="24" t="s">
+        <v>495</v>
+      </c>
+      <c r="X17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="Y17" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="AA17" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC17" s="5">
+        <v>34</v>
       </c>
       <c r="AD17" s="4"/>
       <c r="AE17" s="5" t="s">
@@ -7784,13 +7805,13 @@
         <v>-0.06</v>
       </c>
       <c r="AG17" s="24" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="AH17" s="5">
         <v>-0.2</v>
       </c>
       <c r="AI17" s="24" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
       <c r="AJ17" s="5">
         <v>0.84</v>
@@ -7811,13 +7832,13 @@
         <v>-0.05</v>
       </c>
       <c r="AQ17" s="24" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="AR17" s="5">
         <v>-0.65</v>
       </c>
       <c r="AS17" s="24" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="AT17" s="5">
         <v>0.52</v>
@@ -7840,13 +7861,13 @@
         <v>-0.23</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>371</v>
+        <v>334</v>
       </c>
       <c r="D18" s="5">
         <v>-1.57</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>403</v>
+        <v>366</v>
       </c>
       <c r="F18" s="5">
         <v>0.12</v>
@@ -7873,7 +7894,7 @@
         <v>-0.65</v>
       </c>
       <c r="O18" s="36" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="P18" s="5">
         <v>0.52</v>
@@ -7887,32 +7908,32 @@
       <c r="S18" s="13">
         <v>172</v>
       </c>
-      <c r="U18" s="4" t="s">
+      <c r="U18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="V18" s="4">
-        <v>0.34</v>
-      </c>
-      <c r="W18" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="X18" s="4">
-        <v>1.95</v>
-      </c>
-      <c r="Y18" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="Z18" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="AA18" s="37">
-        <v>26</v>
-      </c>
-      <c r="AB18" s="37">
-        <v>25</v>
-      </c>
-      <c r="AC18" s="37">
-        <v>170</v>
+      <c r="V18" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="W18" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="X18" s="5">
+        <v>1.47</v>
+      </c>
+      <c r="Y18" s="36" t="s">
+        <v>505</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AA18" s="13">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="13">
+        <v>22</v>
+      </c>
+      <c r="AC18" s="13">
+        <v>161</v>
       </c>
       <c r="AE18" s="5" t="s">
         <v>29</v>
@@ -7921,13 +7942,13 @@
         <v>0.01</v>
       </c>
       <c r="AG18" s="24" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="AH18" s="5">
         <v>0.05</v>
       </c>
       <c r="AI18" s="36" t="s">
-        <v>410</v>
+        <v>373</v>
       </c>
       <c r="AJ18" s="5">
         <v>0.96</v>
@@ -7948,13 +7969,13 @@
         <v>-0.03</v>
       </c>
       <c r="AQ18" s="24" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AR18" s="5">
         <v>-0.19</v>
       </c>
       <c r="AS18" s="36" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="AT18" s="5">
         <v>0.85</v>
@@ -7983,7 +8004,7 @@
         <v>0.42</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>404</v>
+        <v>367</v>
       </c>
       <c r="F19" s="5">
         <v>0.67</v>
@@ -8004,13 +8025,13 @@
         <v>-0.06</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N19" s="5">
         <v>-0.23</v>
       </c>
       <c r="O19" s="36" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="P19" s="5">
         <v>0.82</v>
@@ -8028,28 +8049,28 @@
         <v>30</v>
       </c>
       <c r="V19" s="5">
-        <v>0.14000000000000001</v>
+        <v>-0.15</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>167</v>
+        <v>497</v>
       </c>
       <c r="X19" s="5">
-        <v>0.6</v>
+        <v>-0.42</v>
       </c>
       <c r="Y19" s="24" t="s">
-        <v>239</v>
+        <v>506</v>
       </c>
       <c r="Z19" s="5">
-        <v>0.55000000000000004</v>
+        <v>0.68</v>
       </c>
       <c r="AA19" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB19" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AC19" s="5">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="AE19" s="5" t="s">
         <v>30</v>
@@ -8058,13 +8079,13 @@
         <v>-0.13</v>
       </c>
       <c r="AG19" s="24" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="AH19" s="5">
         <v>-0.44</v>
       </c>
       <c r="AI19" s="36" t="s">
-        <v>411</v>
+        <v>374</v>
       </c>
       <c r="AJ19" s="5">
         <v>0.66</v>
@@ -8085,13 +8106,13 @@
         <v>0.37</v>
       </c>
       <c r="AQ19" s="26" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="AR19" s="4">
         <v>3.28</v>
       </c>
       <c r="AS19" s="26" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="AT19" s="4">
         <v>2E-3</v>
@@ -8114,13 +8135,13 @@
         <v>-1.23</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>372</v>
+        <v>335</v>
       </c>
       <c r="D20" s="5">
         <v>-1.34</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>405</v>
+        <v>368</v>
       </c>
       <c r="F20" s="5">
         <v>0.18</v>
@@ -8141,13 +8162,13 @@
         <v>-0.36</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N20" s="5">
         <v>-1.32</v>
       </c>
       <c r="O20" s="36" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="P20" s="5">
         <v>0.19</v>
@@ -8168,25 +8189,25 @@
         <v>0.23</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>168</v>
+        <v>498</v>
       </c>
       <c r="X20" s="5">
-        <v>0.73</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="Y20" s="24" t="s">
-        <v>240</v>
+        <v>507</v>
       </c>
       <c r="Z20" s="5">
-        <v>0.47</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="AA20" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB20" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC20" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AE20" s="5" t="s">
         <v>31</v>
@@ -8195,13 +8216,13 @@
         <v>0.08</v>
       </c>
       <c r="AG20" s="24" t="s">
-        <v>380</v>
+        <v>343</v>
       </c>
       <c r="AH20" s="5">
         <v>0.25</v>
       </c>
       <c r="AI20" s="36" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
       <c r="AJ20" s="5">
         <v>0.81</v>
@@ -8222,13 +8243,13 @@
         <v>-0.05</v>
       </c>
       <c r="AQ20" s="24" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="AR20" s="5">
         <v>-0.13</v>
       </c>
       <c r="AS20" s="36" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="AT20" s="5">
         <v>0.9</v>
@@ -8251,7 +8272,7 @@
         <v>0.33</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="D21" s="22">
         <v>0.42</v>
@@ -8278,7 +8299,7 @@
         <v>0.37</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N21" s="22">
         <v>0.28000000000000003</v>
@@ -8299,16 +8320,19 @@
         <v>34</v>
       </c>
       <c r="V21" s="22">
-        <v>-0.62</v>
+        <v>-0.87</v>
       </c>
       <c r="W21" s="29" t="s">
-        <v>169</v>
+        <v>499</v>
       </c>
       <c r="X21" s="22">
-        <v>-0.99</v>
+        <v>-1.23</v>
+      </c>
+      <c r="Y21" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="Z21" s="22">
-        <v>0.32</v>
+        <v>0.22</v>
       </c>
       <c r="AA21" s="22" t="s">
         <v>54</v>
@@ -8326,7 +8350,7 @@
         <v>-1.83</v>
       </c>
       <c r="AG21" s="30" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="AH21" s="19">
         <v>-3.65</v>
@@ -8354,7 +8378,7 @@
         <v>-2.17</v>
       </c>
       <c r="AQ21" s="29" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="AR21" s="22">
         <v>-1.2</v>
@@ -8380,13 +8404,13 @@
         <v>0.33</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>374</v>
+        <v>337</v>
       </c>
       <c r="D22" s="13">
         <v>0.22</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>406</v>
+        <v>369</v>
       </c>
       <c r="F22" s="13">
         <v>0.83</v>
@@ -8408,13 +8432,13 @@
         <v>-0.09</v>
       </c>
       <c r="M22" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N22" s="13">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="O22" s="36" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="P22" s="13">
         <v>0.95</v>
@@ -8433,19 +8457,19 @@
         <v>55</v>
       </c>
       <c r="V22" s="13">
-        <v>0.05</v>
+        <v>1.31</v>
       </c>
       <c r="W22" s="36" t="s">
-        <v>170</v>
+        <v>500</v>
       </c>
       <c r="X22" s="13">
-        <v>0.06</v>
+        <v>0.62</v>
       </c>
       <c r="Y22" s="36" t="s">
-        <v>241</v>
+        <v>508</v>
       </c>
       <c r="Z22" s="13">
-        <v>0.95</v>
+        <v>0.53</v>
       </c>
       <c r="AA22" s="22" t="s">
         <v>54</v>
@@ -8464,13 +8488,13 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="AG22" s="26" t="s">
-        <v>381</v>
+        <v>344</v>
       </c>
       <c r="AH22" s="4">
         <v>3.63</v>
       </c>
       <c r="AI22" s="4" t="s">
-        <v>412</v>
+        <v>375</v>
       </c>
       <c r="AJ22" s="4">
         <v>2.9999999999999997E-4</v>
@@ -8492,13 +8516,13 @@
         <v>4.08</v>
       </c>
       <c r="AQ22" s="42" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="AR22" s="37">
         <v>2.0299999999999998</v>
       </c>
       <c r="AS22" s="37" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="AT22" s="37">
         <v>0.05</v>
@@ -8521,13 +8545,13 @@
         <v>-0.88</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>375</v>
+        <v>338</v>
       </c>
       <c r="D23" s="13">
         <v>-1.1499999999999999</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>407</v>
+        <v>370</v>
       </c>
       <c r="F23" s="13">
         <v>0.25</v>
@@ -8549,13 +8573,13 @@
         <v>-0.6</v>
       </c>
       <c r="M23" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N23" s="13">
         <v>-0.46</v>
       </c>
       <c r="O23" s="36" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="P23" s="13">
         <v>0.64</v>
@@ -8570,31 +8594,31 @@
         <v>54</v>
       </c>
       <c r="T23" s="22"/>
-      <c r="U23" s="37" t="s">
+      <c r="U23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="V23" s="37">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="W23" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="X23" s="37">
-        <v>1.86</v>
-      </c>
-      <c r="Y23" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z23" s="37">
-        <v>0.06</v>
-      </c>
-      <c r="AA23" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB23" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC23" s="19" t="s">
+      <c r="V23" s="13">
+        <v>1.05</v>
+      </c>
+      <c r="W23" s="36" t="s">
+        <v>501</v>
+      </c>
+      <c r="X23" s="13">
+        <v>1.52</v>
+      </c>
+      <c r="Y23" s="36" t="s">
+        <v>509</v>
+      </c>
+      <c r="Z23" s="13">
+        <v>0.13</v>
+      </c>
+      <c r="AA23" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB23" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC23" s="22" t="s">
         <v>54</v>
       </c>
       <c r="AD23" s="19"/>
@@ -8605,13 +8629,13 @@
         <v>1.97</v>
       </c>
       <c r="AG23" s="42" t="s">
-        <v>382</v>
+        <v>345</v>
       </c>
       <c r="AH23" s="4">
         <v>3.57</v>
       </c>
       <c r="AI23" s="4" t="s">
-        <v>413</v>
+        <v>376</v>
       </c>
       <c r="AJ23" s="4">
         <v>4.0000000000000002E-4</v>
@@ -8633,13 +8657,13 @@
         <v>1.35</v>
       </c>
       <c r="AQ23" s="36" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="AR23" s="13">
         <v>0.68</v>
       </c>
       <c r="AS23" s="36" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="AT23" s="13">
         <v>0.5</v>
@@ -8662,13 +8686,13 @@
         <v>-0.91</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>376</v>
+        <v>339</v>
       </c>
       <c r="D24" s="13">
         <v>-1.1100000000000001</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
       <c r="F24" s="13">
         <v>0.27</v>
@@ -8690,13 +8714,13 @@
         <v>-0.66</v>
       </c>
       <c r="M24" s="36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N24" s="13">
         <v>-0.48</v>
       </c>
       <c r="O24" s="36" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="P24" s="13">
         <v>0.63</v>
@@ -8715,19 +8739,19 @@
         <v>57</v>
       </c>
       <c r="V24" s="13">
-        <v>1.44</v>
+        <v>0.21</v>
       </c>
       <c r="W24" s="36" t="s">
-        <v>172</v>
+        <v>502</v>
       </c>
       <c r="X24" s="13">
-        <v>1.44</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="Y24" s="36" t="s">
-        <v>243</v>
+        <v>510</v>
       </c>
       <c r="Z24" s="13">
-        <v>0.15</v>
+        <v>0.89</v>
       </c>
       <c r="AA24" s="22" t="s">
         <v>54</v>
@@ -8746,13 +8770,13 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="AG24" s="42" t="s">
-        <v>383</v>
+        <v>346</v>
       </c>
       <c r="AH24" s="4">
         <v>4.08</v>
       </c>
       <c r="AI24" s="4" t="s">
-        <v>414</v>
+        <v>377</v>
       </c>
       <c r="AJ24" s="4" t="s">
         <v>59</v>
@@ -8774,13 +8798,13 @@
         <v>2.76</v>
       </c>
       <c r="AQ24" s="36" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="AR24" s="13">
         <v>1.46</v>
       </c>
       <c r="AS24" s="36" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
       <c r="AT24" s="13">
         <v>0.15</v>
@@ -8803,13 +8827,13 @@
         <v>-3.43</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>377</v>
+        <v>340</v>
       </c>
       <c r="D25" s="15">
         <v>-0.72</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>409</v>
+        <v>372</v>
       </c>
       <c r="F25" s="15">
         <v>0.47</v>
@@ -8831,13 +8855,13 @@
         <v>-0.13</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N25" s="15">
         <v>-0.08</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="P25" s="15">
         <v>0.93</v>
@@ -8855,20 +8879,20 @@
       <c r="U25" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="V25" s="15">
-        <v>-0.24</v>
-      </c>
-      <c r="W25" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="X25" s="15">
-        <v>-0.09</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z25" s="15">
-        <v>0.93</v>
+      <c r="V25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="W25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="X25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="AA25" s="15" t="s">
         <v>54</v>
@@ -8887,13 +8911,13 @@
         <v>1.67</v>
       </c>
       <c r="AG25" s="14" t="s">
-        <v>384</v>
+        <v>347</v>
       </c>
       <c r="AH25" s="14">
         <v>2.6</v>
       </c>
       <c r="AI25" s="34" t="s">
-        <v>415</v>
+        <v>378</v>
       </c>
       <c r="AJ25" s="14">
         <v>8.9999999999999993E-3</v>
@@ -8915,13 +8939,13 @@
         <v>2.58</v>
       </c>
       <c r="AQ25" s="25" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="AR25" s="15">
         <v>0.89</v>
       </c>
       <c r="AS25" s="25" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="AT25" s="15">
         <v>0.37</v>
@@ -8976,7 +9000,7 @@
         <v>23</v>
       </c>
       <c r="V27" s="5">
-        <v>1484.69</v>
+        <v>1405.87</v>
       </c>
       <c r="W27" s="5" t="s">
         <v>7</v>
@@ -9008,7 +9032,7 @@
         <v>1.63</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>385</v>
+        <v>348</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>39</v>
@@ -9020,7 +9044,7 @@
         <v>0.72</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="N28" s="5" t="s">
         <v>39</v>
@@ -9029,10 +9053,10 @@
         <v>36</v>
       </c>
       <c r="V28" s="5">
-        <v>0.99</v>
+        <v>0.8</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>197</v>
+        <v>485</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>39</v>
@@ -9056,7 +9080,7 @@
         <v>1.81</v>
       </c>
       <c r="AQ28" s="5" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="AR28" s="5" t="s">
         <v>39</v>
@@ -9233,13 +9257,13 @@
         <v>12</v>
       </c>
       <c r="V31" s="5">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="W31" s="5">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="X31" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AE31" s="5" t="s">
         <v>12</v>
@@ -9298,10 +9322,10 @@
         <v>0</v>
       </c>
       <c r="W32" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="X32" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AE32" s="5" t="s">
         <v>50</v>
@@ -9357,13 +9381,13 @@
         <v>15</v>
       </c>
       <c r="V33" s="5">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="W33" s="5">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="X33" s="5">
-        <v>481</v>
+        <v>420</v>
       </c>
       <c r="AE33" s="5" t="s">
         <v>15</v>
@@ -9590,13 +9614,13 @@
         <v>0.03</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>386</v>
+        <v>349</v>
       </c>
       <c r="D36" s="21">
         <v>0.16</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>416</v>
+        <v>379</v>
       </c>
       <c r="F36" s="21">
         <v>0.87</v>
@@ -9617,13 +9641,13 @@
         <v>-0.09</v>
       </c>
       <c r="M36" s="31" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="N36" s="21">
         <v>-0.72</v>
       </c>
       <c r="O36" s="31" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="P36" s="21">
         <v>0.47</v>
@@ -9641,28 +9665,28 @@
         <v>27</v>
       </c>
       <c r="V36" s="21">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="W36" s="31" t="s">
-        <v>198</v>
+        <v>486</v>
       </c>
       <c r="X36" s="21">
-        <v>-0.79</v>
+        <v>-0.35</v>
       </c>
       <c r="Y36" s="31" t="s">
-        <v>245</v>
+        <v>511</v>
       </c>
       <c r="Z36" s="21">
-        <v>0.43</v>
+        <v>0.73</v>
       </c>
       <c r="AA36" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AB36" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC36" s="5">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="AD36" s="4"/>
       <c r="AE36" s="21" t="s">
@@ -9672,13 +9696,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AG36" s="31" t="s">
-        <v>394</v>
+        <v>357</v>
       </c>
       <c r="AH36" s="21">
         <v>0.41</v>
       </c>
       <c r="AI36" s="31" t="s">
-        <v>425</v>
+        <v>388</v>
       </c>
       <c r="AJ36" s="21">
         <v>0.69</v>
@@ -9699,13 +9723,13 @@
         <v>0.03</v>
       </c>
       <c r="AQ36" s="31" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="AR36" s="21">
         <v>0.14000000000000001</v>
       </c>
       <c r="AS36" s="31" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="AT36" s="21">
         <v>0.89</v>
@@ -9728,13 +9752,13 @@
         <v>-0.12</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
       <c r="D37" s="22">
         <v>-0.63</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>417</v>
+        <v>380</v>
       </c>
       <c r="F37" s="22">
         <v>0.53</v>
@@ -9761,7 +9785,7 @@
         <v>-1.86</v>
       </c>
       <c r="O37" s="30" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="P37" s="19">
         <v>0.06</v>
@@ -9783,25 +9807,25 @@
         <v>0.02</v>
       </c>
       <c r="W37" s="29" t="s">
-        <v>118</v>
+        <v>349</v>
       </c>
       <c r="X37" s="22">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="Y37" s="29" t="s">
-        <v>140</v>
+        <v>512</v>
       </c>
       <c r="Z37" s="22">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="AA37" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AB37" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AC37" s="5">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="AE37" s="22" t="s">
         <v>28</v>
@@ -9810,13 +9834,13 @@
         <v>0.11</v>
       </c>
       <c r="AG37" s="29" t="s">
-        <v>395</v>
+        <v>358</v>
       </c>
       <c r="AH37" s="22">
         <v>0.63</v>
       </c>
       <c r="AI37" s="29" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
       <c r="AJ37" s="22">
         <v>0.53</v>
@@ -9837,13 +9861,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AQ37" s="30" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="AR37" s="19">
         <v>2.41</v>
       </c>
       <c r="AS37" s="30" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="AT37" s="19">
         <v>0.02</v>
@@ -9866,13 +9890,13 @@
         <v>0.02</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D38" s="22">
         <v>0.15</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="F38" s="22">
         <v>0.88</v>
@@ -9893,13 +9917,13 @@
         <v>-0.03</v>
       </c>
       <c r="M38" s="29" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="N38" s="22">
         <v>-0.53</v>
       </c>
       <c r="O38" s="36" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="P38" s="22">
         <v>0.6</v>
@@ -9917,28 +9941,28 @@
         <v>29</v>
       </c>
       <c r="V38" s="22">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="W38" s="29" t="s">
-        <v>199</v>
+        <v>487</v>
       </c>
       <c r="X38" s="22">
-        <v>-0.16</v>
+        <v>-0.37</v>
       </c>
       <c r="Y38" s="36" t="s">
-        <v>246</v>
+        <v>513</v>
       </c>
       <c r="Z38" s="22">
-        <v>0.87</v>
+        <v>0.71</v>
       </c>
       <c r="AA38" s="13">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AB38" s="13">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AC38" s="13">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="AE38" s="22" t="s">
         <v>29</v>
@@ -9947,13 +9971,13 @@
         <v>0.11</v>
       </c>
       <c r="AG38" s="29" t="s">
-        <v>396</v>
+        <v>359</v>
       </c>
       <c r="AH38" s="22">
         <v>0.57999999999999996</v>
       </c>
       <c r="AI38" s="36" t="s">
-        <v>426</v>
+        <v>389</v>
       </c>
       <c r="AJ38" s="22">
         <v>0.56000000000000005</v>
@@ -9980,7 +10004,7 @@
         <v>0.38</v>
       </c>
       <c r="AS38" s="36" t="s">
-        <v>271</v>
+        <v>234</v>
       </c>
       <c r="AT38" s="22">
         <v>0.7</v>
@@ -10003,13 +10027,13 @@
         <v>-0.37</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
       <c r="D39" s="19">
         <v>-2.4900000000000002</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>419</v>
+        <v>382</v>
       </c>
       <c r="F39" s="19">
         <v>0.01</v>
@@ -10037,7 +10061,7 @@
         <v>-0.01</v>
       </c>
       <c r="O39" s="29" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="P39" s="22">
         <v>0.99</v>
@@ -10055,28 +10079,28 @@
         <v>30</v>
       </c>
       <c r="V39" s="22">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="W39" s="29" t="s">
-        <v>118</v>
+        <v>488</v>
       </c>
       <c r="X39" s="22">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="Y39" s="36" t="s">
-        <v>247</v>
+        <v>514</v>
       </c>
       <c r="Z39" s="22">
         <v>0.81</v>
       </c>
       <c r="AA39" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB39" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AC39" s="5">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="AE39" s="22" t="s">
         <v>30</v>
@@ -10085,13 +10109,13 @@
         <v>0.04</v>
       </c>
       <c r="AG39" s="29" t="s">
-        <v>397</v>
+        <v>360</v>
       </c>
       <c r="AH39" s="22">
         <v>0.2</v>
       </c>
       <c r="AI39" s="36" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="AJ39" s="22">
         <v>0.84</v>
@@ -10112,13 +10136,13 @@
         <v>0.08</v>
       </c>
       <c r="AQ39" s="29" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="AR39" s="22">
         <v>0.71</v>
       </c>
       <c r="AS39" s="29" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
       <c r="AT39" s="22">
         <v>0.48</v>
@@ -10141,13 +10165,13 @@
         <v>1.69</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="D40" s="22">
         <v>1.51</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="F40" s="22">
         <v>0.13</v>
@@ -10168,13 +10192,13 @@
         <v>0.04</v>
       </c>
       <c r="M40" s="29" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="N40" s="22">
         <v>0.35</v>
       </c>
       <c r="O40" s="36" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="P40" s="22">
         <v>0.72</v>
@@ -10192,28 +10216,28 @@
         <v>31</v>
       </c>
       <c r="V40" s="22">
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="W40" s="29" t="s">
-        <v>200</v>
+        <v>489</v>
       </c>
       <c r="X40" s="22">
-        <v>1.02</v>
+        <v>1.32</v>
       </c>
       <c r="Y40" s="36" t="s">
-        <v>248</v>
+        <v>515</v>
       </c>
       <c r="Z40" s="22">
-        <v>0.31</v>
+        <v>0.19</v>
       </c>
       <c r="AA40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC40" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AE40" s="22" t="s">
         <v>31</v>
@@ -10222,13 +10246,13 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AG40" s="29" t="s">
-        <v>398</v>
+        <v>361</v>
       </c>
       <c r="AH40" s="22">
         <v>0.75</v>
       </c>
       <c r="AI40" s="36" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="AJ40" s="22">
         <v>0.46</v>
@@ -10249,13 +10273,13 @@
         <v>0.03</v>
       </c>
       <c r="AQ40" s="29" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="AR40" s="22">
         <v>0.05</v>
       </c>
       <c r="AS40" s="36" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="AT40" s="22">
         <v>0.96</v>
@@ -10278,7 +10302,7 @@
         <v>-0.7</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>389</v>
+        <v>352</v>
       </c>
       <c r="D41" s="22">
         <v>-0.85</v>
@@ -10305,7 +10329,7 @@
         <v>-0.55000000000000004</v>
       </c>
       <c r="M41" s="29" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="N41" s="22">
         <v>-0.53</v>
@@ -10326,16 +10350,19 @@
         <v>34</v>
       </c>
       <c r="V41" s="22">
-        <v>0.08</v>
+        <v>0.17</v>
       </c>
       <c r="W41" s="29" t="s">
-        <v>201</v>
+        <v>490</v>
       </c>
       <c r="X41" s="22">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Y41" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="Z41" s="22">
-        <v>0.76</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="AA41" s="22" t="s">
         <v>54</v>
@@ -10353,7 +10380,7 @@
         <v>0.25</v>
       </c>
       <c r="AG41" s="29" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="AH41" s="22">
         <v>0.77</v>
@@ -10380,7 +10407,7 @@
         <v>-2.2999999999999998</v>
       </c>
       <c r="AQ41" s="29" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="AR41" s="22">
         <v>-0.77</v>
@@ -10406,13 +10433,13 @@
         <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>390</v>
+        <v>353</v>
       </c>
       <c r="D42" s="13">
         <v>-2E-3</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>421</v>
+        <v>384</v>
       </c>
       <c r="F42" s="13">
         <v>0.99</v>
@@ -10434,7 +10461,7 @@
         <v>0.33</v>
       </c>
       <c r="M42" s="36" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="N42" s="13">
         <v>0.3</v>
@@ -10459,19 +10486,19 @@
         <v>55</v>
       </c>
       <c r="V42" s="13">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="W42" s="36" t="s">
-        <v>202</v>
+        <v>491</v>
       </c>
       <c r="X42" s="13">
-        <v>1.65</v>
+        <v>1.03</v>
       </c>
       <c r="Y42" s="36" t="s">
-        <v>249</v>
+        <v>516</v>
       </c>
       <c r="Z42" s="13">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AA42" s="22" t="s">
         <v>54</v>
@@ -10490,13 +10517,13 @@
         <v>-0.16</v>
       </c>
       <c r="AG42" s="24" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="AH42" s="5">
         <v>-0.34</v>
       </c>
       <c r="AI42" s="36" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="AJ42" s="5">
         <v>0.73</v>
@@ -10518,13 +10545,13 @@
         <v>-1.27</v>
       </c>
       <c r="AQ42" s="36" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="AR42" s="13">
         <v>-0.39</v>
       </c>
       <c r="AS42" s="36" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="AT42" s="13">
         <v>0.7</v>
@@ -10547,13 +10574,13 @@
         <v>1.32</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>391</v>
+        <v>354</v>
       </c>
       <c r="D43" s="13">
         <v>1.46</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>422</v>
+        <v>385</v>
       </c>
       <c r="F43" s="13">
         <v>0.15</v>
@@ -10575,13 +10602,13 @@
         <v>0.62</v>
       </c>
       <c r="M43" s="36" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="N43" s="13">
         <v>0.57999999999999996</v>
       </c>
       <c r="O43" s="36" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="P43" s="13">
         <v>0.56000000000000005</v>
@@ -10600,19 +10627,19 @@
         <v>56</v>
       </c>
       <c r="V43" s="13">
-        <v>0.01</v>
+        <v>-0.08</v>
       </c>
       <c r="W43" s="36" t="s">
-        <v>203</v>
+        <v>492</v>
       </c>
       <c r="X43" s="13">
-        <v>0.04</v>
+        <v>-0.2</v>
       </c>
       <c r="Y43" s="36" t="s">
-        <v>250</v>
+        <v>517</v>
       </c>
       <c r="Z43" s="13">
-        <v>0.97</v>
+        <v>0.84</v>
       </c>
       <c r="AA43" s="22" t="s">
         <v>54</v>
@@ -10631,13 +10658,13 @@
         <v>-0.3</v>
       </c>
       <c r="AG43" s="36" t="s">
-        <v>399</v>
+        <v>362</v>
       </c>
       <c r="AH43" s="5">
         <v>-0.83</v>
       </c>
       <c r="AI43" s="36" t="s">
-        <v>428</v>
+        <v>391</v>
       </c>
       <c r="AJ43" s="5">
         <v>0.41</v>
@@ -10659,13 +10686,13 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="AQ43" s="36" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="AR43" s="13">
         <v>0.75</v>
       </c>
       <c r="AS43" s="36" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="AT43" s="13">
         <v>0.46</v>
@@ -10688,13 +10715,13 @@
         <v>2.48</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>392</v>
+        <v>355</v>
       </c>
       <c r="D44" s="37">
         <v>2.48</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>423</v>
+        <v>386</v>
       </c>
       <c r="F44" s="37">
         <v>0.01</v>
@@ -10722,7 +10749,7 @@
         <v>0.8</v>
       </c>
       <c r="O44" s="36" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="P44" s="13">
         <v>0.42</v>
@@ -10741,19 +10768,19 @@
         <v>57</v>
       </c>
       <c r="V44" s="13">
-        <v>-0.36</v>
+        <v>-0.34</v>
       </c>
       <c r="W44" s="36" t="s">
-        <v>204</v>
+        <v>493</v>
       </c>
       <c r="X44" s="13">
-        <v>-0.56999999999999995</v>
+        <v>-0.39</v>
       </c>
       <c r="Y44" s="36" t="s">
-        <v>251</v>
+        <v>518</v>
       </c>
       <c r="Z44" s="13">
-        <v>0.56999999999999995</v>
+        <v>0.7</v>
       </c>
       <c r="AA44" s="22" t="s">
         <v>54</v>
@@ -10772,13 +10799,13 @@
         <v>-0.11</v>
       </c>
       <c r="AG44" s="36" t="s">
-        <v>400</v>
+        <v>363</v>
       </c>
       <c r="AH44" s="5">
         <v>-0.28000000000000003</v>
       </c>
       <c r="AI44" s="36" t="s">
-        <v>429</v>
+        <v>392</v>
       </c>
       <c r="AJ44" s="5">
         <v>0.78</v>
@@ -10800,13 +10827,13 @@
         <v>3.41</v>
       </c>
       <c r="AQ44" s="36" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="AR44" s="13">
         <v>1.1299999999999999</v>
       </c>
       <c r="AS44" s="36" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="AT44" s="13">
         <v>0.26</v>
@@ -10829,13 +10856,13 @@
         <v>9.23</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>393</v>
+        <v>356</v>
       </c>
       <c r="D45" s="15">
         <v>1.59</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>424</v>
+        <v>387</v>
       </c>
       <c r="F45" s="15">
         <v>0.11</v>
@@ -10857,13 +10884,13 @@
         <v>0.2</v>
       </c>
       <c r="M45" s="25" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="N45" s="15">
         <v>0.16</v>
       </c>
       <c r="O45" s="25" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="P45" s="15">
         <v>0.87</v>
@@ -10881,20 +10908,20 @@
       <c r="U45" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="V45" s="15">
-        <v>-0.57999999999999996</v>
-      </c>
-      <c r="W45" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="X45" s="15">
-        <v>-0.32</v>
-      </c>
-      <c r="Y45" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="Z45" s="15">
-        <v>0.75</v>
+      <c r="V45" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="W45" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="X45" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y45" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z45" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="AA45" s="15" t="s">
         <v>54</v>
@@ -10913,13 +10940,13 @@
         <v>-0.43</v>
       </c>
       <c r="AG45" s="25" t="s">
-        <v>401</v>
+        <v>364</v>
       </c>
       <c r="AH45" s="15">
         <v>-0.99</v>
       </c>
       <c r="AI45" s="25" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="AJ45" s="15">
         <v>0.32</v>
@@ -10941,13 +10968,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AQ45" s="25" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="AR45" s="15">
         <v>0.53</v>
       </c>
       <c r="AS45" s="25" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="AT45" s="15">
         <v>0.6</v>
@@ -11864,7 +11891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E1601E-514F-6C4E-8014-9481A0BF4F36}">
   <dimension ref="A1:AW97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K2" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -11879,13 +11906,13 @@
   <sheetData>
     <row r="1" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>311</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>273</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="43"/>
@@ -11938,7 +11965,7 @@
     </row>
     <row r="3" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>272</v>
       </c>
       <c r="B3"/>
       <c r="K3" s="19"/>
@@ -12075,7 +12102,7 @@
         <v>0.15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>71</v>
@@ -12111,7 +12138,7 @@
         <v>7</v>
       </c>
       <c r="AB7" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="AG7" s="5" t="s">
         <v>36</v>
@@ -12624,7 +12651,7 @@
         <v>-0.27</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
       <c r="D15" s="13">
         <v>-0.89</v>
@@ -12672,7 +12699,7 @@
         <v>0.03</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>286</v>
+        <v>249</v>
       </c>
       <c r="T15" s="5">
         <v>0.13</v>
@@ -12696,7 +12723,7 @@
         <v>0.27</v>
       </c>
       <c r="AA15" s="26" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="AB15" s="4">
         <v>1.89</v>
@@ -12746,7 +12773,7 @@
         <v>-0.23</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>445</v>
+        <v>408</v>
       </c>
       <c r="D16" s="13">
         <v>-0.38</v>
@@ -12770,7 +12797,7 @@
         <v>-0.09</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="L16">
         <v>-0.32</v>
@@ -12809,7 +12836,7 @@
         <v>0.15</v>
       </c>
       <c r="AA16" s="24" t="s">
-        <v>434</v>
+        <v>397</v>
       </c>
       <c r="AB16" s="5">
         <v>1.35</v>
@@ -12883,7 +12910,7 @@
         <v>-0.13</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="L17">
         <v>-0.44</v>
@@ -12907,7 +12934,7 @@
         <v>0.37</v>
       </c>
       <c r="S17" s="26" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="T17" s="4">
         <v>1.89</v>
@@ -12931,7 +12958,7 @@
         <v>0.13</v>
       </c>
       <c r="AA17" s="24" t="s">
-        <v>435</v>
+        <v>398</v>
       </c>
       <c r="AB17" s="5">
         <v>1.25</v>
@@ -13249,7 +13276,7 @@
         <v>0.16</v>
       </c>
       <c r="K20" s="29" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="L20" s="22">
         <v>0.31</v>
@@ -13273,7 +13300,7 @@
         <v>-0.87</v>
       </c>
       <c r="S20" s="29" t="s">
-        <v>288</v>
+        <v>251</v>
       </c>
       <c r="T20" s="22">
         <v>-1.32</v>
@@ -13297,7 +13324,7 @@
         <v>-2.02</v>
       </c>
       <c r="AA20" s="30" t="s">
-        <v>433</v>
+        <v>396</v>
       </c>
       <c r="AB20" s="19">
         <v>-4.2699999999999996</v>
@@ -13419,7 +13446,7 @@
         <v>3.45</v>
       </c>
       <c r="AA21" s="26" t="s">
-        <v>432</v>
+        <v>395</v>
       </c>
       <c r="AB21" s="4">
         <v>4.82</v>
@@ -13493,7 +13520,7 @@
         <v>-0.38</v>
       </c>
       <c r="K22" s="36" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="L22" s="13">
         <v>-0.7</v>
@@ -13517,7 +13544,7 @@
         <v>1.29</v>
       </c>
       <c r="S22" s="42" t="s">
-        <v>289</v>
+        <v>252</v>
       </c>
       <c r="T22" s="37">
         <v>2.37</v>
@@ -13541,7 +13568,7 @@
         <v>1.96</v>
       </c>
       <c r="AA22" s="42" t="s">
-        <v>431</v>
+        <v>394</v>
       </c>
       <c r="AB22" s="4">
         <v>3.83</v>
@@ -13663,7 +13690,7 @@
         <v>1.94</v>
       </c>
       <c r="AA23" s="42" t="s">
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="AB23" s="4">
         <v>3.78</v>
@@ -13852,7 +13879,7 @@
         <v>256.10000000000002</v>
       </c>
       <c r="C26" t="s">
-        <v>446</v>
+        <v>409</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>23</v>
@@ -13904,7 +13931,7 @@
         <v>0.59</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>36</v>
@@ -13913,7 +13940,7 @@
         <v>0.62</v>
       </c>
       <c r="K27" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="Q27" s="5" t="s">
         <v>36</v>
@@ -13922,7 +13949,7 @@
         <v>0.51</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="Y27" s="5" t="s">
         <v>36</v>
@@ -13931,7 +13958,7 @@
         <v>0.37</v>
       </c>
       <c r="AA27" t="s">
-        <v>349</v>
+        <v>312</v>
       </c>
       <c r="AG27" s="5" t="s">
         <v>36</v>
@@ -14490,7 +14517,7 @@
         <v>-0.08</v>
       </c>
       <c r="S35" s="31" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="T35" s="21">
         <v>-1.07</v>
@@ -14514,7 +14541,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AA35" s="28" t="s">
-        <v>436</v>
+        <v>399</v>
       </c>
       <c r="AB35" s="7">
         <v>0.48</v>
@@ -14588,7 +14615,7 @@
         <v>-0.11</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="L36">
         <v>-1.1000000000000001</v>
@@ -14636,7 +14663,7 @@
         <v>0.1</v>
       </c>
       <c r="AA36" s="32" t="s">
-        <v>437</v>
+        <v>400</v>
       </c>
       <c r="AB36" s="18">
         <v>0.71</v>
@@ -14758,7 +14785,7 @@
         <v>0.1</v>
       </c>
       <c r="AA37" s="32" t="s">
-        <v>438</v>
+        <v>401</v>
       </c>
       <c r="AB37" s="18">
         <v>0.71</v>
@@ -14880,7 +14907,7 @@
         <v>0.02</v>
       </c>
       <c r="AA38" s="32" t="s">
-        <v>439</v>
+        <v>402</v>
       </c>
       <c r="AB38" s="18">
         <v>0.28000000000000003</v>
@@ -15076,7 +15103,7 @@
         <v>-0.28000000000000003</v>
       </c>
       <c r="K40" s="29" t="s">
-        <v>284</v>
+        <v>247</v>
       </c>
       <c r="L40" s="22">
         <v>-0.72</v>
@@ -15100,7 +15127,7 @@
         <v>0.05</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="T40" s="22">
         <v>0.16</v>
@@ -15124,7 +15151,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="AA40" s="32" t="s">
-        <v>440</v>
+        <v>403</v>
       </c>
       <c r="AB40" s="18">
         <v>0.91</v>
@@ -15246,7 +15273,7 @@
         <v>-0.15</v>
       </c>
       <c r="AA41" s="24" t="s">
-        <v>441</v>
+        <v>404</v>
       </c>
       <c r="AB41" s="5">
         <v>-0.3</v>
@@ -15320,7 +15347,7 @@
         <v>0.39</v>
       </c>
       <c r="K42" s="36" t="s">
-        <v>285</v>
+        <v>248</v>
       </c>
       <c r="L42" s="13">
         <v>0.93</v>
@@ -15344,7 +15371,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="S42" s="36" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c r="T42" s="13">
         <v>0.2</v>
@@ -15368,7 +15395,7 @@
         <v>-0.28999999999999998</v>
       </c>
       <c r="AA42" s="36" t="s">
-        <v>442</v>
+        <v>405</v>
       </c>
       <c r="AB42" s="5">
         <v>-0.83</v>
@@ -15490,7 +15517,7 @@
         <v>-0.03</v>
       </c>
       <c r="AA43" s="36" t="s">
-        <v>443</v>
+        <v>406</v>
       </c>
       <c r="AB43" s="5">
         <v>-0.2</v>
@@ -16163,20 +16190,20 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>484</v>
+        <v>447</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -16207,16 +16234,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B5">
-        <v>146.26</v>
+        <v>1069.5</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H5">
         <v>321.39999999999998</v>
@@ -16227,16 +16254,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B6">
-        <v>0.13</v>
+        <v>0.67</v>
       </c>
       <c r="C6" t="s">
-        <v>489</v>
+        <v>522</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H6" s="4">
         <v>5.46</v>
@@ -16294,13 +16321,13 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.9</v>
+        <v>2.23</v>
       </c>
       <c r="C9">
-        <v>0.95</v>
+        <v>1.49</v>
       </c>
       <c r="D9">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -16323,10 +16350,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D10">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
         <v>37</v>
@@ -16346,13 +16373,13 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.31</v>
+        <v>0.15</v>
       </c>
       <c r="C11">
-        <v>0.56000000000000005</v>
+        <v>0.39</v>
       </c>
       <c r="D11">
-        <v>422</v>
+        <v>165</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
@@ -16419,10 +16446,18 @@
       <c r="A14" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="B14" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.41</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="45" t="s">
         <v>70</v>
@@ -16431,7 +16466,7 @@
         <v>0.44</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>491</v>
+        <v>454</v>
       </c>
       <c r="J14" s="21">
         <v>0.4</v>
@@ -16446,19 +16481,19 @@
         <v>34</v>
       </c>
       <c r="B15" s="16">
-        <v>0.3</v>
+        <v>-0.66</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>447</v>
+        <v>524</v>
       </c>
       <c r="D15" s="16">
-        <v>1.82</v>
+        <v>-0.82</v>
       </c>
       <c r="E15" s="16">
-        <v>7.0000000000000007E-2</v>
+        <v>0.41</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>34</v>
@@ -16467,7 +16502,7 @@
         <v>-2.16</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>490</v>
+        <v>453</v>
       </c>
       <c r="J15" s="14">
         <v>-2.34</v>
@@ -16489,16 +16524,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B17">
-        <v>146.26</v>
+        <v>475.98</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H17">
         <v>146.26</v>
@@ -16509,22 +16544,22 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B18">
-        <v>0.13</v>
+        <v>0.45</v>
       </c>
       <c r="C18" t="s">
-        <v>489</v>
+        <v>521</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H18">
         <v>0.13</v>
       </c>
       <c r="I18" t="s">
-        <v>489</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -16576,13 +16611,13 @@
         <v>12</v>
       </c>
       <c r="B21">
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
       <c r="C21">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="D21">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -16605,10 +16640,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
@@ -16628,13 +16663,13 @@
         <v>15</v>
       </c>
       <c r="B23">
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
       <c r="C23">
-        <v>0.33</v>
+        <v>0.23</v>
       </c>
       <c r="D23">
-        <v>422</v>
+        <v>165</v>
       </c>
       <c r="G23" t="s">
         <v>15</v>
@@ -16701,10 +16736,18 @@
       <c r="A26" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="7">
+        <v>-0.04</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="D26" s="21">
+        <v>-0.36</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.72</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="45" t="s">
         <v>70</v>
@@ -16713,7 +16756,7 @@
         <v>0.05</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>485</v>
+        <v>448</v>
       </c>
       <c r="J26" s="21">
         <v>0.52</v>
@@ -16728,16 +16771,16 @@
         <v>34</v>
       </c>
       <c r="B27" s="16">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="D27" s="16">
-        <v>-0.04</v>
+        <v>0.67</v>
       </c>
       <c r="E27" s="16">
-        <v>0.97</v>
+        <v>0.5</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>39</v>
@@ -16749,7 +16792,7 @@
         <v>0.13</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>486</v>
+        <v>449</v>
       </c>
       <c r="J27" s="16">
         <v>0.36</v>
@@ -16778,13 +16821,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>492</v>
+        <v>455</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -16815,7 +16858,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B5">
         <v>334.17</v>
@@ -16824,7 +16867,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H5">
         <v>313.77999999999997</v>
@@ -16835,22 +16878,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B6">
         <v>0.23</v>
       </c>
       <c r="C6" t="s">
-        <v>513</v>
+        <v>476</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H6" s="4">
         <v>3.92</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>502</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -17031,7 +17074,7 @@
         <v>-0.16</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>514</v>
+        <v>477</v>
       </c>
       <c r="D14" s="21">
         <v>-0.41</v>
@@ -17047,7 +17090,7 @@
         <v>-0.09</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>503</v>
+        <v>466</v>
       </c>
       <c r="J14" s="21">
         <v>-0.16</v>
@@ -17065,7 +17108,7 @@
         <v>0.27</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>515</v>
+        <v>478</v>
       </c>
       <c r="D15" s="16">
         <v>0.48</v>
@@ -17083,7 +17126,7 @@
         <v>1.36</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>504</v>
+        <v>467</v>
       </c>
       <c r="J15" s="14">
         <v>1.98</v>
@@ -17105,16 +17148,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B17">
         <v>68.27</v>
       </c>
       <c r="C17" t="s">
-        <v>510</v>
+        <v>473</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H17">
         <v>201.5</v>
@@ -17125,16 +17168,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B18">
         <v>0.15</v>
       </c>
       <c r="C18" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H18">
         <v>0.01</v>
@@ -17321,7 +17364,7 @@
         <v>-0.12</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>511</v>
+        <v>474</v>
       </c>
       <c r="D26" s="47">
         <v>-1.95</v>
@@ -17339,7 +17382,7 @@
         <v>0.09</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>500</v>
+        <v>463</v>
       </c>
       <c r="J26" s="21">
         <v>0.59</v>
@@ -17357,7 +17400,7 @@
         <v>-0.13</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>512</v>
+        <v>475</v>
       </c>
       <c r="D27" s="16">
         <v>-0.39</v>
@@ -17375,7 +17418,7 @@
         <v>-0.05</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>501</v>
+        <v>464</v>
       </c>
       <c r="J27" s="16">
         <v>-7.0000000000000007E-2</v>
@@ -17396,21 +17439,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6C0B71-6C7E-C94B-9EF8-31E2F1C25E26}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -17463,7 +17506,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B5">
         <v>1592.83</v>
@@ -17472,7 +17515,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H5">
         <v>614.58000000000004</v>
@@ -17481,16 +17524,16 @@
         <v>7</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="N5">
-        <v>146.26</v>
+        <v>923.09</v>
       </c>
       <c r="O5" t="s">
         <v>7</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="T5">
         <v>402.76</v>
@@ -17501,34 +17544,34 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B6">
         <v>0.15</v>
       </c>
       <c r="C6" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H6" s="5">
         <v>1.07</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>518</v>
+        <v>481</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="N6">
-        <v>0.13</v>
+        <v>0.46</v>
       </c>
       <c r="O6" t="s">
-        <v>489</v>
+        <v>521</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="T6" s="5">
         <v>0.92</v>
@@ -17653,10 +17696,10 @@
         <v>0.9</v>
       </c>
       <c r="O9">
-        <v>0.95</v>
+        <v>0.31</v>
       </c>
       <c r="P9">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="S9" t="s">
         <v>12</v>
@@ -17706,7 +17749,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="S10" t="s">
         <v>37</v>
@@ -17750,13 +17793,13 @@
         <v>15</v>
       </c>
       <c r="N11">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="O11">
         <v>0.56000000000000005</v>
       </c>
       <c r="P11">
-        <v>422</v>
+        <v>161</v>
       </c>
       <c r="S11" t="s">
         <v>15</v>
@@ -17871,7 +17914,7 @@
         <v>-0.27</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
       <c r="D14" s="21">
         <v>-0.88</v>
@@ -17887,7 +17930,7 @@
         <v>0.06</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>519</v>
+        <v>482</v>
       </c>
       <c r="J14" s="21">
         <v>0.39</v>
@@ -17899,10 +17942,18 @@
       <c r="M14" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="7"/>
+      <c r="N14" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="O14" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="P14" s="21">
+        <v>1.68</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0.09</v>
+      </c>
       <c r="R14" s="7"/>
       <c r="S14" s="45" t="s">
         <v>70</v>
@@ -17911,7 +17962,7 @@
         <v>0.09</v>
       </c>
       <c r="U14" s="28" t="s">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="V14" s="21">
         <v>0.96</v>
@@ -17929,7 +17980,7 @@
         <v>-0.23</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>445</v>
+        <v>408</v>
       </c>
       <c r="D15" s="16">
         <v>-0.38</v>
@@ -17947,7 +17998,7 @@
         <v>-0.32</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>520</v>
+        <v>483</v>
       </c>
       <c r="J15" s="16">
         <v>-1.03</v>
@@ -17962,19 +18013,19 @@
         <v>34</v>
       </c>
       <c r="N15" s="16">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>447</v>
+        <v>528</v>
       </c>
       <c r="P15" s="16">
-        <v>1.82</v>
+        <v>0.68</v>
       </c>
       <c r="Q15" s="16">
-        <v>7.0000000000000007E-2</v>
+        <v>0.5</v>
       </c>
       <c r="R15" s="16" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="S15" s="16" t="s">
         <v>34</v>
@@ -17983,7 +18034,7 @@
         <v>-0.16</v>
       </c>
       <c r="U15" s="27" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="V15" s="16">
         <v>-0.96</v>
@@ -18011,16 +18062,16 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B17">
         <v>256.10000000000002</v>
       </c>
       <c r="C17" t="s">
-        <v>446</v>
+        <v>409</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H17">
         <v>307.62</v>
@@ -18029,16 +18080,16 @@
         <v>7</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="N17">
-        <v>146.26</v>
+        <v>561.57000000000005</v>
       </c>
       <c r="O17" t="s">
         <v>7</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="T17">
         <v>175.27</v>
@@ -18049,40 +18100,40 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B18">
         <v>0.59</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="H18">
         <v>0.24</v>
       </c>
       <c r="I18" t="s">
-        <v>513</v>
+        <v>476</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="N18">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>489</v>
+        <v>525</v>
       </c>
       <c r="S18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="T18">
         <v>0.88</v>
       </c>
       <c r="U18" t="s">
-        <v>497</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -18198,13 +18249,13 @@
         <v>12</v>
       </c>
       <c r="N21">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="O21">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="P21">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="S21" t="s">
         <v>12</v>
@@ -18251,10 +18302,10 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="P22">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="S22" t="s">
         <v>37</v>
@@ -18298,13 +18349,13 @@
         <v>15</v>
       </c>
       <c r="N23">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="O23">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="P23">
-        <v>422</v>
+        <v>161</v>
       </c>
       <c r="S23" t="s">
         <v>15</v>
@@ -18435,7 +18486,7 @@
         <v>-0.04</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>516</v>
+        <v>479</v>
       </c>
       <c r="J26" s="21">
         <v>-0.28000000000000003</v>
@@ -18447,10 +18498,18 @@
       <c r="M26" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="7"/>
+      <c r="N26" s="7">
+        <v>-0.04</v>
+      </c>
+      <c r="O26" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="P26" s="21">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="R26" s="7"/>
       <c r="S26" s="45" t="s">
         <v>70</v>
@@ -18459,7 +18518,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U26" s="28" t="s">
-        <v>495</v>
+        <v>458</v>
       </c>
       <c r="V26" s="21">
         <v>1.37</v>
@@ -18495,7 +18554,7 @@
         <v>0.1</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="J27" s="16">
         <v>0.49</v>
@@ -18510,16 +18569,16 @@
         <v>34</v>
       </c>
       <c r="N27" s="16">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="O27" s="27" t="s">
-        <v>469</v>
+        <v>526</v>
       </c>
       <c r="P27" s="16">
-        <v>-0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q27" s="16">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="R27" s="16" t="s">
         <v>39</v>
@@ -18531,7 +18590,7 @@
         <v>0.08</v>
       </c>
       <c r="U27" s="27" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="V27" s="16">
         <v>0.94</v>
@@ -18560,13 +18619,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>494</v>
+        <v>457</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -18586,7 +18645,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B5">
         <v>658.46</v>
@@ -18597,13 +18656,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>508</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -18706,7 +18765,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>509</v>
+        <v>472</v>
       </c>
       <c r="D14" s="21">
         <v>-0.02</v>
@@ -18743,7 +18802,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="B17">
         <v>361.16</v>
@@ -18754,13 +18813,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="B18">
         <v>0.27</v>
       </c>
       <c r="C18" t="s">
-        <v>507</v>
+        <v>470</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -18863,7 +18922,7 @@
         <v>-0.06</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>505</v>
+        <v>468</v>
       </c>
       <c r="D26" s="21">
         <v>-0.4</v>
@@ -18881,7 +18940,7 @@
         <v>0.13</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>506</v>
+        <v>469</v>
       </c>
       <c r="D27" s="16">
         <v>0.52</v>

</xml_diff>